<commit_message>
collected and analysed historical data in preparation for data inputs and model calibration
</commit_message>
<xml_diff>
--- a/code/COSA_Data/electricity_price_data.xlsx
+++ b/code/COSA_Data/electricity_price_data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="337">
   <si>
     <t>Rohdaten Tariferhebung ElCom 2020</t>
   </si>
@@ -999,12 +999,54 @@
   </si>
   <si>
     <t>DATA FROM historical_data.xlsx file and electricity_price_XX series (incl. taxes)</t>
+  </si>
+  <si>
+    <t>fit_high</t>
+  </si>
+  <si>
+    <t>fit_low</t>
+  </si>
+  <si>
+    <t>ewz_high_large</t>
+  </si>
+  <si>
+    <t>ewz_low_large</t>
+  </si>
+  <si>
+    <t>ewz_high_small</t>
+  </si>
+  <si>
+    <t>ewz_low_small</t>
+  </si>
+  <si>
+    <t>ewz_solarsplit_fee</t>
+  </si>
+  <si>
+    <t>ratio_high_low</t>
+  </si>
+  <si>
+    <t>2018_high</t>
+  </si>
+  <si>
+    <t>2018_low</t>
+  </si>
+  <si>
+    <t>av_price = (6/24) * low_price + (18/24) * high_price</t>
+  </si>
+  <si>
+    <t>high_price = ratio_high_low &amp; low_price</t>
+  </si>
+  <si>
+    <t>low_price = av_price / ((6/24) + (18/24) * ratio_high_low)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -1094,7 +1136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1120,9 +1162,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1130,6 +1169,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9110,7 +9153,7 @@
       <c r="I203" s="3"/>
     </row>
     <row r="204" spans="1:9" ht="28">
-      <c r="A204" s="11"/>
+      <c r="A204" s="16"/>
       <c r="B204" s="6" t="s">
         <v>72</v>
       </c>
@@ -9128,7 +9171,7 @@
       </c>
     </row>
     <row r="205" spans="1:9" ht="28">
-      <c r="A205" s="11"/>
+      <c r="A205" s="16"/>
       <c r="B205" s="6" t="s">
         <v>73</v>
       </c>
@@ -9257,7 +9300,7 @@
       <c r="A213" s="5"/>
     </row>
     <row r="214" spans="1:5" ht="28">
-      <c r="A214" s="11"/>
+      <c r="A214" s="16"/>
       <c r="B214" s="6" t="s">
         <v>72</v>
       </c>
@@ -9272,7 +9315,7 @@
       </c>
     </row>
     <row r="215" spans="1:5" ht="28">
-      <c r="A215" s="11"/>
+      <c r="A215" s="16"/>
       <c r="B215" s="6" t="s">
         <v>73</v>
       </c>
@@ -9380,7 +9423,7 @@
       <c r="A222" s="5"/>
     </row>
     <row r="223" spans="1:5" ht="28">
-      <c r="A223" s="11"/>
+      <c r="A223" s="16"/>
       <c r="B223" s="6" t="s">
         <v>72</v>
       </c>
@@ -9395,7 +9438,7 @@
       </c>
     </row>
     <row r="224" spans="1:5" ht="28">
-      <c r="A224" s="11"/>
+      <c r="A224" s="16"/>
       <c r="B224" s="6" t="s">
         <v>73</v>
       </c>
@@ -9511,10 +9554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK186"/>
+  <dimension ref="A1:AR186"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4:AK14"/>
+      <selection activeCell="AJ18" sqref="AJ18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -9530,34 +9573,46 @@
     <col min="26" max="26" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="99.54296875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="8.90625" customWidth="1"/>
+    <col min="41" max="41" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:44">
       <c r="AC1" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="2" spans="1:37">
+      <c r="AL1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44">
       <c r="A2" t="s">
         <v>122</v>
       </c>
       <c r="Q2" t="s">
         <v>282</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="U2" s="12" t="s">
         <v>286</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14" t="s">
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="3" spans="1:37">
+      <c r="AL2" t="s">
+        <v>334</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -9585,16 +9640,16 @@
       <c r="V3" t="s">
         <v>285</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="Z3" s="15" t="s">
+      <c r="Z3" s="14" t="s">
         <v>305</v>
       </c>
-      <c r="AA3" s="15" t="s">
+      <c r="AA3" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="AB3" s="15" t="s">
+      <c r="AB3" s="14" t="s">
         <v>318</v>
       </c>
       <c r="AC3" s="1">
@@ -9624,8 +9679,24 @@
       <c r="AK3" s="1">
         <v>2018</v>
       </c>
-    </row>
-    <row r="4" spans="1:37">
+      <c r="AL3" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AP3" s="17">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AQ3">
+        <f>AP3/AP4</f>
+        <v>1.910112359550562</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44">
       <c r="O4" t="s">
         <v>14</v>
       </c>
@@ -9644,17 +9715,17 @@
       <c r="V4" t="s">
         <v>285</v>
       </c>
-      <c r="Y4" s="14" t="s">
+      <c r="Y4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="Z4" s="14" t="s">
+      <c r="Z4" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="AA4" s="16" t="s">
+      <c r="AA4" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="AB4" s="14">
-        <f>VLOOKUP(Y4,$O$4:$Q$18,3,0)</f>
+      <c r="AB4" s="13">
+        <f t="shared" ref="AB4:AB14" si="0">VLOOKUP(Y4,$O$4:$Q$18,3,0)</f>
         <v>1.6</v>
       </c>
       <c r="AC4">
@@ -9684,8 +9755,22 @@
       <c r="AK4">
         <v>23.463214285714297</v>
       </c>
-    </row>
-    <row r="5" spans="1:37">
+      <c r="AL4" s="17">
+        <f>AM4*$AQ$7</f>
+        <v>26.123991163475711</v>
+      </c>
+      <c r="AM4" s="17">
+        <f>AK4/(0.25+0.75*$AQ$7)</f>
+        <v>15.480883652430052</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AP4" s="17">
+        <v>4.4499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44">
       <c r="A5" t="s">
         <v>124</v>
       </c>
@@ -9707,17 +9792,17 @@
       <c r="V5" t="s">
         <v>285</v>
       </c>
-      <c r="Y5" s="14" t="s">
+      <c r="Y5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Z5" s="14" t="s">
+      <c r="Z5" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="AA5" s="16" t="s">
+      <c r="AA5" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="AB5" s="14">
-        <f>VLOOKUP(Y5,$O$4:$Q$18,3,0)</f>
+      <c r="AB5" s="13">
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="AC5">
@@ -9747,8 +9832,26 @@
       <c r="AK5">
         <v>23.075494285714299</v>
       </c>
-    </row>
-    <row r="6" spans="1:37">
+      <c r="AL5" s="17">
+        <f t="shared" ref="AL5:AL14" si="1">AM5*$AQ$7</f>
+        <v>25.692302916053034</v>
+      </c>
+      <c r="AM5" s="17">
+        <f t="shared" ref="AM5:AM14" si="2">AK5/(0.25+0.75*$AQ$7)</f>
+        <v>15.225068394698095</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="AP5" s="17">
+        <v>0.06</v>
+      </c>
+      <c r="AQ5">
+        <f>AP5/AP6</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44">
       <c r="O6" t="s">
         <v>16</v>
       </c>
@@ -9770,17 +9873,17 @@
       <c r="V6" t="s">
         <v>285</v>
       </c>
-      <c r="Y6" s="14" t="s">
+      <c r="Y6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="Z6" s="14" t="s">
+      <c r="Z6" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="AA6" s="16" t="s">
+      <c r="AA6" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="AB6" s="14">
-        <f>VLOOKUP(Y6,$O$4:$Q$18,3,0)</f>
+      <c r="AB6" s="13">
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="AC6">
@@ -9810,8 +9913,22 @@
       <c r="AK6">
         <v>22.919585714285734</v>
       </c>
-    </row>
-    <row r="7" spans="1:37">
+      <c r="AL6" s="17">
+        <f t="shared" si="1"/>
+        <v>25.518713991163498</v>
+      </c>
+      <c r="AM6" s="17">
+        <f t="shared" si="2"/>
+        <v>15.122200883652443</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="AP6" s="17">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -9833,17 +9950,17 @@
       <c r="V7" t="s">
         <v>285</v>
       </c>
-      <c r="Y7" s="14" t="s">
+      <c r="Y7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="Z7" s="14" t="s">
+      <c r="Z7" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="AA7" s="16" t="s">
+      <c r="AA7" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="AB7" s="14">
-        <f>VLOOKUP(Y7,$O$4:$Q$18,3,0)</f>
+      <c r="AB7" s="13">
+        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
       <c r="AC7">
@@ -9873,8 +9990,30 @@
       <c r="AK7">
         <v>22.921637142857097</v>
       </c>
-    </row>
-    <row r="8" spans="1:37">
+      <c r="AL7" s="17">
+        <f t="shared" si="1"/>
+        <v>25.520998055964604</v>
+      </c>
+      <c r="AM7" s="17">
+        <f t="shared" si="2"/>
+        <v>15.12355440353458</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="AP7" s="17">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="AQ7" s="13">
+        <f>AP7/AP8</f>
+        <v>1.6875</v>
+      </c>
+      <c r="AR7">
+        <f>0.25*AP8+0.75*AP7</f>
+        <v>0.21825</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44">
       <c r="O8" t="s">
         <v>18</v>
       </c>
@@ -9896,17 +10035,17 @@
       <c r="V8" t="s">
         <v>284</v>
       </c>
-      <c r="Y8" s="14" t="s">
+      <c r="Y8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="Z8" s="14" t="s">
+      <c r="Z8" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="AA8" s="16" t="s">
+      <c r="AA8" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="AB8" s="14">
-        <f>VLOOKUP(Y8,$O$4:$Q$18,3,0)</f>
+      <c r="AB8" s="13">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="AC8">
@@ -9936,8 +10075,22 @@
       <c r="AK8">
         <v>20.757695604395632</v>
       </c>
-    </row>
-    <row r="9" spans="1:37">
+      <c r="AL8" s="17">
+        <f t="shared" si="1"/>
+        <v>23.111661085306476</v>
+      </c>
+      <c r="AM8" s="17">
+        <f t="shared" si="2"/>
+        <v>13.695799161663098</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="AP8" s="17">
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -9962,17 +10115,17 @@
       <c r="V9" t="s">
         <v>285</v>
       </c>
-      <c r="Y9" s="14" t="s">
+      <c r="Y9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="Z9" s="14" t="s">
+      <c r="Z9" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="AA9" s="16" t="s">
+      <c r="AA9" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="AB9" s="14">
-        <f>VLOOKUP(Y9,$O$4:$Q$18,3,0)</f>
+      <c r="AB9" s="13">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="AC9">
@@ -10002,8 +10155,22 @@
       <c r="AK9">
         <v>16.953210857142903</v>
       </c>
-    </row>
-    <row r="10" spans="1:37">
+      <c r="AL9" s="17">
+        <f t="shared" si="1"/>
+        <v>18.875739923416837</v>
+      </c>
+      <c r="AM9" s="17">
+        <f t="shared" si="2"/>
+        <v>11.18562365832109</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="AP9" s="17">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44">
       <c r="O10" t="s">
         <v>20</v>
       </c>
@@ -10022,17 +10189,17 @@
       <c r="V10" t="s">
         <v>285</v>
       </c>
-      <c r="Y10" s="14" t="s">
+      <c r="Y10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="Z10" s="14" t="s">
+      <c r="Z10" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="AA10" s="16" t="s">
+      <c r="AA10" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="AB10" s="14">
-        <f>VLOOKUP(Y10,$O$4:$Q$18,3,0)</f>
+      <c r="AB10" s="13">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AC10">
@@ -10062,8 +10229,16 @@
       <c r="AK10">
         <v>25.080637500000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:37">
+      <c r="AL10" s="17">
+        <f t="shared" si="1"/>
+        <v>27.924833505154641</v>
+      </c>
+      <c r="AM10" s="17">
+        <f t="shared" si="2"/>
+        <v>16.548049484536083</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44">
       <c r="A11" t="s">
         <v>128</v>
       </c>
@@ -10085,17 +10260,17 @@
       <c r="V11" t="s">
         <v>285</v>
       </c>
-      <c r="Y11" s="14" t="s">
+      <c r="Y11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="Z11" s="14" t="s">
+      <c r="Z11" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="AA11" s="16" t="s">
+      <c r="AA11" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="AB11" s="14">
-        <f>VLOOKUP(Y11,$O$4:$Q$18,3,0)</f>
+      <c r="AB11" s="13">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="AC11">
@@ -10125,8 +10300,16 @@
       <c r="AK11">
         <v>24.911009999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:37">
+      <c r="AL11" s="17">
+        <f t="shared" si="1"/>
+        <v>27.735969896907211</v>
+      </c>
+      <c r="AM11" s="17">
+        <f t="shared" si="2"/>
+        <v>16.436130309278347</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44">
       <c r="O12" t="s">
         <v>22</v>
       </c>
@@ -10145,17 +10328,17 @@
       <c r="V12" t="s">
         <v>285</v>
       </c>
-      <c r="Y12" s="14" t="s">
+      <c r="Y12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="Z12" s="14" t="s">
+      <c r="Z12" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="AA12" s="16" t="s">
+      <c r="AA12" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="AB12" s="14">
-        <f>VLOOKUP(Y12,$O$4:$Q$18,3,0)</f>
+      <c r="AB12" s="13">
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="AC12">
@@ -10185,8 +10368,16 @@
       <c r="AK12">
         <v>25.381300000000032</v>
       </c>
-    </row>
-    <row r="13" spans="1:37">
+      <c r="AL12" s="17">
+        <f t="shared" si="1"/>
+        <v>28.259591752577354</v>
+      </c>
+      <c r="AM12" s="17">
+        <f t="shared" si="2"/>
+        <v>16.746424742268061</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -10211,17 +10402,17 @@
       <c r="V13" t="s">
         <v>285</v>
       </c>
-      <c r="Y13" s="14" t="s">
+      <c r="Y13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="Z13" s="14" t="s">
+      <c r="Z13" s="13" t="s">
         <v>315</v>
       </c>
-      <c r="AA13" s="16" t="s">
+      <c r="AA13" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="AB13" s="14">
-        <f>VLOOKUP(Y13,$O$4:$Q$18,3,0)</f>
+      <c r="AB13" s="13">
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="AC13">
@@ -10251,8 +10442,16 @@
       <c r="AK13">
         <v>23.332343399999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:37">
+      <c r="AL13" s="17">
+        <f t="shared" si="1"/>
+        <v>25.978279249484537</v>
+      </c>
+      <c r="AM13" s="17">
+        <f t="shared" si="2"/>
+        <v>15.394535851546392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44">
       <c r="B14" t="s">
         <v>130</v>
       </c>
@@ -10274,17 +10473,17 @@
       <c r="V14" t="s">
         <v>284</v>
       </c>
-      <c r="Y14" s="14" t="s">
+      <c r="Y14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="Z14" s="14" t="s">
+      <c r="Z14" s="13" t="s">
         <v>316</v>
       </c>
-      <c r="AA14" s="16" t="s">
+      <c r="AA14" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="AB14" s="14">
-        <f>VLOOKUP(Y14,$O$4:$Q$18,3,0)</f>
+      <c r="AB14" s="13">
+        <f t="shared" si="0"/>
         <v>7500</v>
       </c>
       <c r="AC14">
@@ -10314,8 +10513,16 @@
       <c r="AK14">
         <v>18.536480383564523</v>
       </c>
-    </row>
-    <row r="15" spans="1:37">
+      <c r="AL14" s="17">
+        <f t="shared" si="1"/>
+        <v>20.638555478607923</v>
+      </c>
+      <c r="AM14" s="17">
+        <f t="shared" si="2"/>
+        <v>12.230255098434325</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44">
       <c r="B15" t="s">
         <v>131</v>
       </c>
@@ -10338,7 +10545,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="43.5">
+    <row r="16" spans="1:44" ht="43.5">
       <c r="C16" t="s">
         <v>134</v>
       </c>
@@ -10357,8 +10564,11 @@
       <c r="R16" t="s">
         <v>301</v>
       </c>
-      <c r="S16" s="12" t="s">
+      <c r="S16" s="11" t="s">
         <v>304</v>
+      </c>
+      <c r="AL16" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -10896,7 +11106,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" ht="43.5">
-      <c r="E83" s="12" t="s">
+      <c r="E83" s="11" t="s">
         <v>175</v>
       </c>
     </row>

</xml_diff>